<commit_message>
new code updated session
</commit_message>
<xml_diff>
--- a/winners.xlsx
+++ b/winners.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="5">
   <si>
     <t>Ticket Number</t>
   </si>
@@ -22,13 +22,13 @@
     <t>Prize</t>
   </si>
   <si>
-    <t>Mixture Grinder (Yasuda)</t>
-  </si>
-  <si>
     <t>Electric Jug (Yasuda)</t>
   </si>
   <si>
     <t>Iron (Yasuda)</t>
+  </si>
+  <si>
+    <t>Mixture Grinder (Yasuda)</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +402,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>15426</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -410,23 +410,23 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>11084</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>11084</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>11084</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -434,15 +434,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>10276</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>11406</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -450,15 +450,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>15617</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>15617</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -466,23 +466,23 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>15617</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>18550</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>18550</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -490,15 +490,15 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>21935</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>11037</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -506,15 +506,15 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>10568</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>10568</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>10568</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -530,15 +530,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>17547</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>17865</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -546,15 +546,15 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>13042</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>17027</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -562,39 +562,39 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>16800</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>11004</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>22317</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>17307</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>14254</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -602,55 +602,55 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>19542</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>19542</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>19542</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>19542</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>19542</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>10083</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>10083</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -658,23 +658,23 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>10083</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>22205</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>10083</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -682,34 +682,1074 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>22205</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>10083</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>22205</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>11157</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>15</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>23</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>19</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>23</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>24</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>15</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>14</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>8</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>14</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>24</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>15</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <v>14</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <v>24</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <v>8</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <v>15</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <v>22</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <v>19</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <v>14</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <v>24</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <v>8</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <v>15</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <v>22</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102">
+        <v>9</v>
+      </c>
+      <c r="B102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103">
+        <v>9</v>
+      </c>
+      <c r="B103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104">
+        <v>9</v>
+      </c>
+      <c r="B104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106">
+        <v>9</v>
+      </c>
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108">
+        <v>9</v>
+      </c>
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110">
+        <v>6</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111">
+        <v>9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113">
+        <v>6</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114">
+        <v>9</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116">
+        <v>6</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117">
+        <v>12</v>
+      </c>
+      <c r="B117" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118">
+        <v>9</v>
+      </c>
+      <c r="B118" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120">
+        <v>6</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121">
+        <v>12</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122">
+        <v>12</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123">
+        <v>9</v>
+      </c>
+      <c r="B123" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125">
+        <v>6</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126">
+        <v>12</v>
+      </c>
+      <c r="B126" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127">
+        <v>12</v>
+      </c>
+      <c r="B127" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128">
+        <v>9</v>
+      </c>
+      <c r="B128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130">
+        <v>6</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131">
+        <v>12</v>
+      </c>
+      <c r="B131" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132">
+        <v>12</v>
+      </c>
+      <c r="B132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133">
+        <v>18</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134">
+        <v>9</v>
+      </c>
+      <c r="B134" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136">
+        <v>6</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137">
+        <v>12</v>
+      </c>
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138">
+        <v>12</v>
+      </c>
+      <c r="B138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139">
+        <v>18</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140">
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141">
+        <v>1</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142">
+        <v>6</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143">
+        <v>12</v>
+      </c>
+      <c r="B143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144">
+        <v>12</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145">
+        <v>18</v>
+      </c>
+      <c r="B145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146">
+        <v>13</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147">
+        <v>9</v>
+      </c>
+      <c r="B147" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149">
+        <v>6</v>
+      </c>
+      <c r="B149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150">
+        <v>12</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151">
+        <v>12</v>
+      </c>
+      <c r="B151" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152">
+        <v>18</v>
+      </c>
+      <c r="B152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153">
+        <v>13</v>
+      </c>
+      <c r="B153" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154">
+        <v>9</v>
+      </c>
+      <c r="B154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156">
+        <v>6</v>
+      </c>
+      <c r="B156" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157">
+        <v>12</v>
+      </c>
+      <c r="B157" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158">
+        <v>12</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159">
+        <v>18</v>
+      </c>
+      <c r="B159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160">
+        <v>13</v>
+      </c>
+      <c r="B160" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161">
+        <v>11</v>
+      </c>
+      <c r="B161" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162">
+        <v>9</v>
+      </c>
+      <c r="B162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="B163" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164">
+        <v>6</v>
+      </c>
+      <c r="B164" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165">
+        <v>12</v>
+      </c>
+      <c r="B165" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166">
+        <v>12</v>
+      </c>
+      <c r="B166" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167">
+        <v>18</v>
+      </c>
+      <c r="B167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168">
+        <v>13</v>
+      </c>
+      <c r="B168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169">
+        <v>11</v>
+      </c>
+      <c r="B169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170">
+        <v>11</v>
+      </c>
+      <c r="B170" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>